<commit_message>
Added How Systems Work
</commit_message>
<xml_diff>
--- a/docs/GKMetroWebDesign.xlsx
+++ b/docs/GKMetroWebDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>Microsoft</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>LinuxBasics.aspx</t>
+  </si>
+  <si>
+    <t>How Systems Work</t>
+  </si>
+  <si>
+    <t>Learn Product Management</t>
   </si>
 </sst>
 </file>
@@ -763,14 +769,34 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1020,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1242,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>